<commit_message>
Update Carol Bell Quote 101802.xlsx
rays changes. Made from an invoice to a bid. Missing description.
</commit_message>
<xml_diff>
--- a/Carol Bell Quote 101802.xlsx
+++ b/Carol Bell Quote 101802.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MainMain1\Downloads\Github\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\raymo\OneDrive\Documents\GitHub\ATO-Contracting-LLC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BC7C2555-FEB6-43A3-A205-F3B9ACD4E21A}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="11" documentId="8_{BC7C2555-FEB6-43A3-A205-F3B9ACD4E21A}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{240AF312-6419-4452-8F4B-FDAE9C229B45}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7485" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t>Date</t>
   </si>
@@ -42,9 +42,6 @@
     <t>Description</t>
   </si>
   <si>
-    <t>Current Balance Due</t>
-  </si>
-  <si>
     <t>Thank You for Your Business!</t>
   </si>
   <si>
@@ -84,9 +81,6 @@
     <t xml:space="preserve">  Sharmain Harris • 262‐344-7779 • P.O Box 1226 Kenosha, WI 53140</t>
   </si>
   <si>
-    <t>Original Balance</t>
-  </si>
-  <si>
     <t xml:space="preserve">raymond.k.roberts@gmail.com </t>
   </si>
   <si>
@@ -99,32 +93,29 @@
     <t>Quote 101801</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Remit to</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">:
+    <t>Description: Painting of assigned areas</t>
+  </si>
+  <si>
+    <t>Materials: Customer providing paint</t>
+  </si>
+  <si>
+    <t>Contractor responsible for all necessary tools and equipment to perfrom</t>
+  </si>
+  <si>
+    <t>scope of work</t>
+  </si>
+  <si>
+    <t>Bid Amount</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                                 Estimate valid for 30 days</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
 Carol Bell
 2717 26th Ave.
 Kenosha, WI 53140
 </t>
-    </r>
-  </si>
-  <si>
-    <t>Description: Painting of assigned areas</t>
   </si>
 </sst>
 </file>
@@ -136,7 +127,7 @@
     <numFmt numFmtId="164" formatCode="m/d/yy;@"/>
     <numFmt numFmtId="165" formatCode="[$-409]mmm\-yy;@"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -185,13 +176,6 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -562,7 +546,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="69">
+  <cellXfs count="70">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -759,6 +743,9 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1103,7 +1090,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D22" sqref="D22"/>
+      <selection pane="bottomLeft" activeCell="C8" sqref="C8:C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.140625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1125,7 +1112,7 @@
     <row r="2" spans="2:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B2" s="55"/>
       <c r="C2" s="49" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D2" s="37"/>
       <c r="E2" s="1"/>
@@ -1136,7 +1123,7 @@
     <row r="3" spans="2:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B3" s="56"/>
       <c r="C3" s="47" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D3" s="37"/>
       <c r="E3" s="26"/>
@@ -1147,7 +1134,7 @@
     <row r="4" spans="2:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B4" s="56"/>
       <c r="C4" s="48" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D4" s="37"/>
       <c r="E4" s="10"/>
@@ -1166,7 +1153,7 @@
     </row>
     <row r="6" spans="2:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" s="53" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C6" s="38"/>
       <c r="D6" s="39"/>
@@ -1177,7 +1164,7 @@
     </row>
     <row r="7" spans="2:8" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B7" s="40" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C7" s="41"/>
       <c r="D7" s="42"/>
@@ -1185,7 +1172,7 @@
     <row r="8" spans="2:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="64"/>
       <c r="C8" s="62" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="D8" s="60"/>
     </row>
@@ -1238,7 +1225,7 @@
       <c r="A18" s="3"/>
       <c r="B18" s="35"/>
       <c r="C18" s="45" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D18" s="36" t="s">
         <v>1</v>
@@ -1263,7 +1250,7 @@
       <c r="A21" s="3"/>
       <c r="B21" s="34"/>
       <c r="C21" s="44" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D21" s="32">
         <v>2000</v>
@@ -1287,21 +1274,29 @@
     <row r="24" spans="1:14" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="3"/>
       <c r="B24" s="34"/>
-      <c r="C24" s="8"/>
-      <c r="D24" s="32"/>
+      <c r="C24" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="D24" s="32">
+        <v>0</v>
+      </c>
       <c r="E24" s="3"/>
     </row>
     <row r="25" spans="1:14" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="3"/>
       <c r="B25" s="34"/>
-      <c r="C25" s="7"/>
+      <c r="C25" s="69" t="s">
+        <v>22</v>
+      </c>
       <c r="D25" s="32"/>
       <c r="E25" s="3"/>
     </row>
     <row r="26" spans="1:14" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="3"/>
       <c r="B26" s="34"/>
-      <c r="C26" s="7"/>
+      <c r="C26" s="69" t="s">
+        <v>23</v>
+      </c>
       <c r="D26" s="32"/>
       <c r="E26" s="3"/>
     </row>
@@ -1348,7 +1343,7 @@
     <row r="32" spans="1:14" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A32" s="3"/>
       <c r="B32" s="46" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="C32" s="8"/>
       <c r="D32" s="32">
@@ -1364,14 +1359,11 @@
     </row>
     <row r="33" spans="1:14" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A33" s="3"/>
-      <c r="B33" s="15" t="s">
-        <v>3</v>
-      </c>
-      <c r="C33" s="16"/>
-      <c r="D33" s="54">
-        <f>SUM(D32:D32)</f>
-        <v>2000</v>
-      </c>
+      <c r="B33" s="15"/>
+      <c r="C33" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="D33" s="54"/>
       <c r="E33" s="3"/>
       <c r="J33" s="27"/>
       <c r="K33" s="58"/>
@@ -1389,7 +1381,7 @@
       <c r="A35" s="3"/>
       <c r="B35" s="3"/>
       <c r="C35" s="9" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D35" s="3"/>
       <c r="E35" s="3"/>
@@ -1449,7 +1441,7 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="66" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B1" s="66"/>
       <c r="C1" s="66"/>
@@ -1461,7 +1453,7 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="67" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B2" s="67"/>
       <c r="C2" s="67"/>
@@ -1473,7 +1465,7 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="68" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B3" s="67"/>
       <c r="C3" s="67"/>
@@ -1513,23 +1505,23 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B7" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" s="13" t="s">
         <v>6</v>
-      </c>
-      <c r="B8" s="13" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="12" t="s">
         <v>8</v>
-      </c>
-      <c r="B9" s="12" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
@@ -1549,7 +1541,7 @@
         <v>2</v>
       </c>
       <c r="C12" s="17" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
@@ -1618,7 +1610,7 @@
     <row r="25" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A25" s="8"/>
       <c r="B25" s="23" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C25" s="24">
         <f>SUM(C13:C23)</f>

</xml_diff>